<commit_message>
create new xlsx file
</commit_message>
<xml_diff>
--- a/file-example.xlsx
+++ b/file-example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\One Drive\OneDrive\Vincent\Vincent Lab\github tutorials\Working with data in JavaScript\Working with XLSX in JavaScript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e412cede43275eb/Code/Personal/Vários/excelErate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6958C767-68F9-4DAE-89E6-48C9462DD496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_87DB871281D25A46975A0FD6628D520E9761D542" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="37">
   <si>
     <t>First Name</t>
   </si>
@@ -44,6 +44,9 @@
     <t>Id</t>
   </si>
   <si>
+    <t>New Column</t>
+  </si>
+  <si>
     <t>Dulce</t>
   </si>
   <si>
@@ -120,6 +123,15 @@
   </si>
   <si>
     <t>Weiland</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>22/09/2020</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -155,9 +167,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -176,9 +187,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -216,7 +227,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -322,7 +333,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -464,7 +475,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -472,18 +483,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="10.125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,219 +511,247 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>1562</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>25</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>43023</v>
       </c>
       <c r="G3">
         <v>1582</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>36</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>43023</v>
       </c>
       <c r="G4">
         <v>2587</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>25</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>43023</v>
       </c>
       <c r="G5">
         <v>3549</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6">
         <v>2468</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G7">
         <v>2554</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <v>3598</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>2456</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>6548</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11">
+        <v>1600</v>
+      </c>
+      <c r="H11" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:H2 A1:G1 A6:H10 A5:E5 G5:H5 A4:E4 G4:H4 A3:E3 G3:H3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H11" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -726,14 +760,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="10.125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -760,22 +789,22 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>1562</v>
@@ -783,21 +812,21 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>25</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>42598</v>
       </c>
       <c r="G3">
@@ -806,21 +835,21 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>36</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>42598</v>
       </c>
       <c r="G4">
@@ -829,21 +858,21 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>25</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>42598</v>
       </c>
       <c r="G5">
@@ -852,21 +881,21 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>58</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>42598</v>
       </c>
       <c r="G6">
@@ -875,22 +904,22 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G7">
         <v>2554</v>
@@ -898,22 +927,22 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <v>3598</v>
@@ -921,22 +950,22 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>2456</v>
@@ -944,22 +973,22 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>6548</v>
@@ -968,7 +997,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G2 A7:G10 A6:E6 G6 A5:E5 G5 A4:E4 G4 A3:E3 G3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G10" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>